<commit_message>
somehow datanya dah rapi
</commit_message>
<xml_diff>
--- a/gempa2012.xlsx
+++ b/gempa2012.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student2014\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Student2014\Documents\GitHub\DDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,13 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
-  <si>
-    <t>Nama Provinsi</t>
-  </si>
-  <si>
-    <t>Jumlah Kejadian - Jumlah</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>PEMERINTAH ACEH</t>
   </si>
@@ -45,9 +39,6 @@
     <t>MALUKU</t>
   </si>
   <si>
-    <t>PAPUA BARAT</t>
-  </si>
-  <si>
     <t>SUMATERA UTARA</t>
   </si>
   <si>
@@ -60,9 +51,6 @@
     <t>Kepri</t>
   </si>
   <si>
-    <t>Sumbar</t>
-  </si>
-  <si>
     <t>JAMBI</t>
   </si>
   <si>
@@ -106,9 +94,6 @@
   </si>
   <si>
     <t>KALIMANTAN TIMUR</t>
-  </si>
-  <si>
-    <t>Kalsel</t>
   </si>
   <si>
     <t>GORONTALO</t>
@@ -509,324 +494,276 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C36"/>
+  <dimension ref="A1:B33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C36"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B14" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.375" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>7</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>0</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>0</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>0</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="B13" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>0</v>
+      </c>
+      <c r="B14" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>0</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>0</v>
+      </c>
+      <c r="B16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>0</v>
+      </c>
+      <c r="B18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
         <v>3</v>
       </c>
-      <c r="B9">
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0</v>
+      </c>
+      <c r="B22" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>0</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>0</v>
+      </c>
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
         <v>1</v>
       </c>
-      <c r="C9" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <v>0</v>
-      </c>
-      <c r="C10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B14">
-        <v>0</v>
-      </c>
-      <c r="C14" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="B27" t="s">
         <v>4</v>
       </c>
-      <c r="B15">
-        <v>2</v>
-      </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B17">
-        <v>0</v>
-      </c>
-      <c r="C17" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B18">
-        <v>0</v>
-      </c>
-      <c r="C18" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B20">
-        <v>0</v>
-      </c>
-      <c r="C20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
         <v>5</v>
       </c>
-      <c r="B21">
-        <v>2</v>
-      </c>
-      <c r="C21" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B22">
-        <v>0</v>
-      </c>
-      <c r="C22" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B23">
-        <v>0</v>
-      </c>
-      <c r="C23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B24">
-        <v>0</v>
-      </c>
-      <c r="C24" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B25">
-        <v>0</v>
-      </c>
-      <c r="C25" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B26">
-        <v>0</v>
-      </c>
-      <c r="C26" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B27">
-        <v>0</v>
-      </c>
-      <c r="C27" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B28">
-        <v>0</v>
-      </c>
-      <c r="C28" t="s">
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B29">
-        <v>0</v>
-      </c>
-      <c r="C29" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>0</v>
+      </c>
+      <c r="B33" t="s">
         <v>32</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>6</v>
-      </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B31">
-        <v>0</v>
-      </c>
-      <c r="C31" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B32">
-        <v>0</v>
-      </c>
-      <c r="C32" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B33">
-        <v>0</v>
-      </c>
-      <c r="C33" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>7</v>
-      </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>8</v>
-      </c>
-      <c r="B35">
-        <v>1</v>
-      </c>
-      <c r="C35" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B36">
-        <v>0</v>
-      </c>
-      <c r="C36" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>